<commit_message>
Updated Results to include averages
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="98">
   <si>
     <t xml:space="preserve">Window: </t>
   </si>
@@ -31,6 +31,9 @@
     <t>Accuracy</t>
   </si>
   <si>
+    <t>Project Accuracy:</t>
+  </si>
+  <si>
     <t>2023-09-24,2025-03-22</t>
   </si>
   <si>
@@ -43,9 +46,15 @@
     <t>3 / 3</t>
   </si>
   <si>
+    <t>Top 3 Correct:</t>
+  </si>
+  <si>
     <t>- face_swapper.py -&gt; 0.79</t>
   </si>
   <si>
+    <t>Total Predictions:</t>
+  </si>
+  <si>
     <t>- core.py -&gt; 0.62</t>
   </si>
   <si>
@@ -293,6 +302,9 @@
   </si>
   <si>
     <t>- english.py -&gt; 0.80</t>
+  </si>
+  <si>
+    <t>Averages</t>
   </si>
 </sst>
 </file>
@@ -556,6 +568,7 @@
     <col customWidth="1" min="1" max="1" width="29.88"/>
     <col customWidth="1" min="2" max="2" width="31.0"/>
     <col customWidth="1" min="3" max="3" width="40.0"/>
+    <col customWidth="1" min="8" max="8" width="14.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -577,38 +590,53 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2">
         <v>0.43</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.46</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1"/>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -619,19 +647,19 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2">
         <v>0.02</v>
@@ -640,14 +668,14 @@
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -656,19 +684,19 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F10" s="2">
         <v>0.02</v>
@@ -678,14 +706,14 @@
     <row r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -694,19 +722,19 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F14" s="2">
         <v>0.04</v>
@@ -715,14 +743,14 @@
     <row r="15">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1"/>
     </row>
@@ -731,19 +759,19 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F18" s="2">
         <v>0.18</v>
@@ -753,14 +781,14 @@
     <row r="19">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1"/>
     </row>
@@ -770,19 +798,19 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F22" s="2">
         <v>0.0</v>
@@ -793,19 +821,19 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F24" s="2">
         <v>0.0</v>
@@ -816,19 +844,19 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F26" s="2">
         <v>0.0</v>
@@ -839,19 +867,19 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F28" s="2">
         <v>0.57</v>
@@ -860,14 +888,14 @@
     <row r="29">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1"/>
     </row>
     <row r="30">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C30" s="1"/>
     </row>
@@ -876,19 +904,19 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F32" s="2">
         <v>0.27</v>
@@ -897,14 +925,14 @@
     <row r="33">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row r="34">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C34" s="1"/>
     </row>
@@ -913,19 +941,19 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F36" s="2">
         <v>0.21</v>
@@ -934,14 +962,14 @@
     <row r="37">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C37" s="1"/>
     </row>
     <row r="38">
       <c r="A38" s="1"/>
       <c r="B38" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C38" s="1"/>
     </row>
@@ -950,19 +978,19 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F40" s="2">
         <v>0.27</v>
@@ -970,13 +998,13 @@
     </row>
     <row r="41">
       <c r="B41" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42">
       <c r="B42" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C42" s="1"/>
     </row>
@@ -985,19 +1013,19 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F44" s="2">
         <v>0.18</v>
@@ -1005,13 +1033,13 @@
     </row>
     <row r="45">
       <c r="B45" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C45" s="1"/>
     </row>
     <row r="46">
       <c r="B46" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C46" s="1"/>
     </row>
@@ -1020,19 +1048,19 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F48" s="2">
         <v>0.25</v>
@@ -1040,13 +1068,13 @@
     </row>
     <row r="49">
       <c r="B49" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50">
       <c r="B50" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C50" s="1"/>
     </row>
@@ -1055,19 +1083,19 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F52" s="2">
         <v>0.33</v>
@@ -1075,13 +1103,13 @@
     </row>
     <row r="53">
       <c r="B53" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C53" s="1"/>
     </row>
     <row r="54">
       <c r="B54" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C54" s="1"/>
     </row>
@@ -1090,19 +1118,19 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F56" s="2">
         <v>0.27</v>
@@ -1110,13 +1138,13 @@
     </row>
     <row r="57">
       <c r="B57" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C57" s="1"/>
     </row>
     <row r="58">
       <c r="B58" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C58" s="1"/>
     </row>
@@ -1125,19 +1153,19 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="D60" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F60" s="2">
         <v>0.21</v>
@@ -1145,13 +1173,13 @@
     </row>
     <row r="61">
       <c r="B61" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62">
       <c r="B62" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C62" s="1"/>
     </row>
@@ -1160,19 +1188,19 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F64" s="2">
         <v>0.5</v>
@@ -1180,13 +1208,13 @@
     </row>
     <row r="65">
       <c r="B65" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C65" s="1"/>
     </row>
     <row r="66">
       <c r="B66" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C66" s="1"/>
     </row>
@@ -1195,19 +1223,19 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="D68" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F68" s="2">
         <v>1.0</v>
@@ -1215,13 +1243,13 @@
     </row>
     <row r="69">
       <c r="B69" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C69" s="1"/>
     </row>
     <row r="70">
       <c r="B70" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C70" s="1"/>
     </row>
@@ -1230,19 +1258,19 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F72" s="2">
         <v>0.0</v>
@@ -1253,19 +1281,19 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F74" s="2">
         <v>0.25</v>
@@ -1273,12 +1301,23 @@
     </row>
     <row r="75">
       <c r="B75" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="D78" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="E78" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>